<commit_message>
update output rnaseq computation
</commit_message>
<xml_diff>
--- a/templates/dataplant/4COM01_RNASeq.xlsx
+++ b/templates/dataplant/4COM01_RNASeq.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\source\repos\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\GitHub\Swate-templates_FORK\templates\dataplant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC96F489-128C-44ED-A460-2BE8FEA473A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46B530D-FF25-4FE0-A5D2-AE6DCBFCD3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="19110" windowHeight="12450" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="2340" windowWidth="22785" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4COM01_RNASeq" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="129">
   <si>
     <t>Source Name</t>
   </si>
@@ -520,12 +520,15 @@
   <si>
     <t>Authors Role Term Source REF</t>
   </si>
+  <si>
+    <t>Derived Data File</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -547,12 +550,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -685,7 +682,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -723,6 +720,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,7 +775,7 @@
     <tableColumn id="24" xr3:uid="{D9EF39FD-6C34-45E7-BB66-0E47D62F2287}" name="Parameter [Processed data file format]"/>
     <tableColumn id="25" xr3:uid="{4F08F69F-150F-4C24-8CF1-DB5CA334C705}" name="Term Source REF (NFDI4PSO:0000027)"/>
     <tableColumn id="26" xr3:uid="{937F41BB-46A8-40D7-BA19-6EAA289C307B}" name="Term Accession Number (NFDI4PSO:0000027)"/>
-    <tableColumn id="27" xr3:uid="{47E29D49-E345-471B-B28D-74992C57C833}" name="Data File Name"/>
+    <tableColumn id="2" xr3:uid="{010FC165-1DFE-496A-A994-5082DE452C3C}" name="Derived Data File"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1081,7 +1079,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="617" row="2">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="3">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="709" row="2">
@@ -1114,36 +1112,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="46.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="45.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.85546875" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="26.85546875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="48.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="41" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
@@ -1223,7 +1223,7 @@
         <v>22</v>
       </c>
       <c r="Z1" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
@@ -1272,6 +1272,7 @@
       <c r="Y2" t="s">
         <v>118</v>
       </c>
+      <c r="Z2" s="13"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K3" t="s">
@@ -1292,6 +1293,7 @@
       <c r="Y3" t="s">
         <v>118</v>
       </c>
+      <c r="Z3" s="13"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K4" t="s">
@@ -1312,6 +1314,7 @@
       <c r="Y4" t="s">
         <v>118</v>
       </c>
+      <c r="Z4" s="13"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
@@ -1323,6 +1326,7 @@
       <c r="M5" t="s">
         <v>118</v>
       </c>
+      <c r="Z5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1336,7 +1340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B11AFC42-7216-4420-8824-56B92332BA6B}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>

</xml_diff>